<commit_message>
Added SP schema in config
</commit_message>
<xml_diff>
--- a/examples/etl_example_empty.xlsx
+++ b/examples/etl_example_empty.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincechavez/Work/UMA_DATA/ETL_AUTOMATION/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE9B1E6-0D20-234A-9C6E-CC753821D9B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A8BBCA-1584-1D4C-8F08-B0D6ABB6B1EE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>SOURCE_SERVER</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>SOURCE_EXCLUDED_COLUMNS</t>
+  </si>
+  <si>
+    <t>STORED_PROCEDURE_SCHEMA</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,16 +525,16 @@
     <col min="16" max="16" width="30" customWidth="1"/>
     <col min="17" max="17" width="31.1640625" customWidth="1"/>
     <col min="18" max="18" width="33.6640625" customWidth="1"/>
-    <col min="19" max="19" width="31.1640625" customWidth="1"/>
-    <col min="20" max="20" width="25.5" customWidth="1"/>
-    <col min="21" max="21" width="33.6640625" customWidth="1"/>
-    <col min="22" max="22" width="31.33203125" customWidth="1"/>
-    <col min="23" max="23" width="31.5" customWidth="1"/>
-    <col min="24" max="24" width="14.33203125" customWidth="1"/>
-    <col min="25" max="25" width="15.83203125" customWidth="1"/>
+    <col min="19" max="20" width="31.1640625" customWidth="1"/>
+    <col min="21" max="21" width="25.5" customWidth="1"/>
+    <col min="22" max="22" width="33.6640625" customWidth="1"/>
+    <col min="23" max="23" width="31.33203125" customWidth="1"/>
+    <col min="24" max="24" width="31.5" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,21 +593,24 @@
         <v>22</v>
       </c>
       <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>